<commit_message>
Cycle 2 Budget Update
</commit_message>
<xml_diff>
--- a/docs/Cycle 2/Budget - Cycle 2.xlsx
+++ b/docs/Cycle 2/Budget - Cycle 2.xlsx
@@ -201,18 +201,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -227,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -261,11 +255,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,24 +625,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="F4" s="23">
-        <v>0</v>
-      </c>
-      <c r="G4" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F4" s="7">
+        <v>22.9</v>
+      </c>
+      <c r="G4" s="8">
+        <f t="shared" si="0"/>
+        <v>22.9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1257,7 +1246,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="11">
         <f>SUBTOTAL(109,'Senior Design Costs '!$G$3:$G$36)</f>
-        <v>217.95</v>
+        <v>240.85</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>